<commit_message>
Added notes and user stories for Print 2
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Project tracking.xlsx
+++ b/ProjectDocuments/Project tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian Ramirez\Documents\SLU\Fall 2021\Princ Of Software Deve\ProjectDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71A0F3F7-922C-4196-9B1B-0B1CB395E143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4896C2-2465-44B4-9348-105EE1CD85D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A5DF588-7268-4165-B066-E7B86B099B0A}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{1A5DF588-7268-4165-B066-E7B86B099B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Story Number</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>As a system admin, I would like to develop the back end in Python and link it with JavaScript</t>
+  </si>
+  <si>
+    <t>As a user, I would like to received context spell checking</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>As a user, I would like to receive spellchecking wihtout having to click a submit button</t>
   </si>
 </sst>
 </file>
@@ -403,16 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C175DEEB-3CA0-4EDF-B550-A8B769980655}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.6640625" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -451,6 +463,31 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
only few changes to project tracking spreadsheet
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Project tracking.xlsx
+++ b/ProjectDocuments/Project tracking.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian Ramirez\Documents\SLU\Fall 2021\Princ Of Software Deve\ProjectDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4896C2-2465-44B4-9348-105EE1CD85D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234C8F85-BE24-4868-9009-6D534546576D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{1A5DF588-7268-4165-B066-E7B86B099B0A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1A5DF588-7268-4165-B066-E7B86B099B0A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="User stories" sheetId="1" r:id="rId1"/>
+    <sheet name="Bug Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Story Number</t>
   </si>
@@ -57,21 +58,116 @@
     <t>As a system admin, I would like to develop the back end in Python and link it with JavaScript</t>
   </si>
   <si>
-    <t>As a user, I would like to received context spell checking</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>As a user, I would like to receive spellchecking wihtout having to click a submit button</t>
+    <t>As a user, I want to be able to replace a word by right-clicking on the word and a menu showing different choices.</t>
+  </si>
+  <si>
+    <t>As a user, I would like to received context spell checking, not only by dictionary</t>
+  </si>
+  <si>
+    <t>As a user, I want to have an ideal user experience by using a well designed application.</t>
+  </si>
+  <si>
+    <t>Bug Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Priorities</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>There is little to none impact in user experience and functionality</t>
+  </si>
+  <si>
+    <t>There is some impact in the user experience but not application functionality</t>
+  </si>
+  <si>
+    <t>There is a considerate impact in user experience and/or functionality</t>
+  </si>
+  <si>
+    <t>Functionality is in jeopardy, user may not be able to get accurate spell checking</t>
+  </si>
+  <si>
+    <t>Assigned to a Sprint</t>
+  </si>
+  <si>
+    <t>Development Completed</t>
+  </si>
+  <si>
+    <t>Pull Request Created</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Node is triggering an error when the array that contains the words is empty.</t>
+  </si>
+  <si>
+    <t>As a user, I would like to receive spell checking without having to click a submit button</t>
+  </si>
+  <si>
+    <t>Created by</t>
+  </si>
+  <si>
+    <t>Julian Ramirez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kimaya Gandhi </t>
+  </si>
+  <si>
+    <t>Manasa Gade</t>
+  </si>
+  <si>
+    <t>Sai Priyatham</t>
+  </si>
+  <si>
+    <t>Reported by</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>When user is typing in the div, sometimes it adds a space after the last word.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,13 +195,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -415,38 +558,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C175DEEB-3CA0-4EDF-B550-A8B769980655}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="94.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -457,39 +601,292 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B148856F-19EA-451E-96CF-949CCD22049A}">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1 D3:D1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{B4E7B3DC-CC76-42E5-9F9E-FF90389281F6}">
+      <formula1>$L$16:$L$20</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{6567E61F-D9D4-4F08-9F86-6433696444D7}">
+      <formula1>$L$6:$L$9</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576 G2:G1048576" xr:uid="{1F199A80-2CA0-4D32-ABD8-F04060EE7666}">
+      <formula1>$L$24:$L$27</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new bugs to spreadsheet
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Project tracking.xlsx
+++ b/ProjectDocuments/Project tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian Ramirez\Documents\SLU\Fall 2021\Princ Of Software Deve\ProjectDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234C8F85-BE24-4868-9009-6D534546576D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C284B64C-7E2A-48B4-BCA2-C82C937E462A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1A5DF588-7268-4165-B066-E7B86B099B0A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1A5DF588-7268-4165-B066-E7B86B099B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Story Number</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>When user is typing in the div, sometimes it adds a space after the last word.</t>
+  </si>
+  <si>
+    <t>Numbers are being flagged as incorrect.</t>
+  </si>
+  <si>
+    <t>Words with dashes are not processing correctly and obstructing the logic.</t>
   </si>
 </sst>
 </file>
@@ -560,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C175DEEB-3CA0-4EDF-B550-A8B769980655}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,15 +698,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B148856F-19EA-451E-96CF-949CCD22049A}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="65.21875" customWidth="1"/>
     <col min="4" max="4" width="10.109375" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" style="3" customWidth="1"/>
@@ -777,7 +783,45 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4</v>
+      </c>
+    </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4</v>
+      </c>
       <c r="L5" t="s">
         <v>15</v>
       </c>

</xml_diff>